<commit_message>
Never forget to push
</commit_message>
<xml_diff>
--- a/RandXY3 (many geometrics).xlsx
+++ b/RandXY3 (many geometrics).xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omare\PycharmProjects\Crytal Detector BA Trial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C968CA-C493-491E-81B7-0FC3A7C18C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525FB75F-3375-4A2F-A61D-B22586FB1F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{72A45E1A-9903-429A-A719-26FC432BF437}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{72A45E1A-9903-429A-A719-26FC432BF437}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,12 +58,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -77,8 +84,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -165,12 +176,108 @@
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:srgbClr val="0070C0"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="0070C0"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-2516-470F-BB6C-C1A209EC7B8F}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="0070C0"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-2516-470F-BB6C-C1A209EC7B8F}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="0070C0"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-2516-470F-BB6C-C1A209EC7B8F}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="0070C0"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-2516-470F-BB6C-C1A209EC7B8F}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$100</c:f>
@@ -184,7 +291,7 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10</c:v>
@@ -193,7 +300,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>30</c:v>
@@ -220,16 +327,16 @@
                   <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>60</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>66</c:v>
@@ -238,22 +345,34 @@
                   <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>66</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>68</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>66</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>63</c:v>
+                  <c:v>7.07</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>60</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>58</c:v>
+                  <c:v>-7.07</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-7.07</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7.07</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -271,7 +390,7 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>20</c:v>
@@ -280,7 +399,7 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>40</c:v>
@@ -307,40 +426,52 @@
                   <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>73</c:v>
-                </c:pt>
                 <c:pt idx="16">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>70</c:v>
-                </c:pt>
                 <c:pt idx="21">
-                  <c:v>67</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>64</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>64</c:v>
+                  <c:v>7.07</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>67</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>70</c:v>
+                  <c:v>7.07</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-7.07</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-7.07</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1105,10 +1236,10 @@
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1453,10 +1584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C982590-4A3F-4B25-84D2-602B1DA6D40D}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1487,10 +1618,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>43</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1510,34 +1641,34 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>24</v>
+      <c r="A7" s="1">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>30</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>33</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>27</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>43</v>
       </c>
     </row>
@@ -1583,10 +1714,10 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B16">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -1594,23 +1725,23 @@
         <v>63</v>
       </c>
       <c r="B17">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B18">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B19">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -1618,7 +1749,7 @@
         <v>66</v>
       </c>
       <c r="B20">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -1626,55 +1757,87 @@
         <v>63</v>
       </c>
       <c r="B21">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B22">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B23">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>66</v>
-      </c>
-      <c r="B24">
-        <v>64</v>
+      <c r="A24" s="2">
+        <v>12</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>63</v>
-      </c>
-      <c r="B25">
-        <v>64</v>
+      <c r="A25" s="2">
+        <v>7.07</v>
+      </c>
+      <c r="B25" s="2">
+        <v>7.07</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>60</v>
-      </c>
-      <c r="B26">
-        <v>67</v>
+      <c r="A26" s="2">
+        <v>0</v>
+      </c>
+      <c r="B26" s="2">
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>58</v>
-      </c>
-      <c r="B27">
-        <v>70</v>
+      <c r="A27" s="2">
+        <v>-7.07</v>
+      </c>
+      <c r="B27" s="2">
+        <v>7.07</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>-12</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>-7.07</v>
+      </c>
+      <c r="B29" s="2">
+        <v>-7.07</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>0</v>
+      </c>
+      <c r="B30" s="2">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>7.07</v>
+      </c>
+      <c r="B31" s="2">
+        <v>-7.07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A few addons to the Calssifier
</commit_message>
<xml_diff>
--- a/RandXY3 (many geometrics).xlsx
+++ b/RandXY3 (many geometrics).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omare\PycharmProjects\Crytal Detector BA Trial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525FB75F-3375-4A2F-A61D-B22586FB1F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E579A7DB-8379-4C86-8CCC-3F2CB2C86CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{72A45E1A-9903-429A-A719-26FC432BF437}"/>
   </bookViews>
@@ -374,6 +374,18 @@
                 <c:pt idx="29">
                   <c:v>7.07</c:v>
                 </c:pt>
+                <c:pt idx="30">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -472,6 +484,18 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>-7.07</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>82.5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>77.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1584,10 +1608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C982590-4A3F-4B25-84D2-602B1DA6D40D}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1840,6 +1864,38 @@
         <v>-7.07</v>
       </c>
     </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>10</v>
+      </c>
+      <c r="B32" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>5</v>
+      </c>
+      <c r="B33" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="B34" s="2">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="B35" s="2">
+        <v>77.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>